<commit_message>
added empirical calculation to Arduino code
I put in the empirical function generated from Matlab. The highest
order poly I was able to get was 3. Any higher and it completely
failed. I think this may be due to a significant rounding error as the
larger degrees had larger numbers.
</commit_message>
<xml_diff>
--- a/MatlabProjectCode/EmpiricalData.xlsx
+++ b/MatlabProjectCode/EmpiricalData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Desktop/1010Project/ME1010/MatlabProjectCode/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,6 +77,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,17 +410,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -421,7 +431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11</v>
       </c>
@@ -432,7 +442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -443,7 +453,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -454,7 +464,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
@@ -465,7 +475,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>48</v>
       </c>
@@ -476,7 +486,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>54</v>
       </c>
@@ -487,7 +497,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>61</v>
       </c>
@@ -498,7 +508,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>70</v>
       </c>
@@ -509,7 +519,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>76</v>
       </c>
@@ -520,7 +530,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>85</v>
       </c>
@@ -531,7 +541,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>92</v>
       </c>
@@ -544,10 +554,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>